<commit_message>
Fixed alternative start codons
</commit_message>
<xml_diff>
--- a/Codon optimization/data_formatted.xlsx
+++ b/Codon optimization/data_formatted.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dennis/Documents/MATLAB/iGEM/Sci-Phi-Software-Tool/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CF45F5-597A-3A42-9655-5EFD987C85E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="412">
   <si>
     <t>combined1</t>
   </si>
@@ -1263,8 +1257,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1278,7 +1272,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1293,27 +1287,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1613,1399 +1603,1458 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BM7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:BM7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
-    <col min="2" max="21" width="12.6640625" customWidth="1"/>
-    <col min="22" max="22" width="10.6640625" customWidth="1"/>
-    <col min="23" max="37" width="12.6640625" customWidth="1"/>
-    <col min="38" max="38" width="10.6640625" customWidth="1"/>
-    <col min="39" max="65" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="true"/>
+    <col min="2" max="2" width="12.7109375" customWidth="true"/>
+    <col min="22" max="22" width="10.7109375" customWidth="true"/>
+    <col min="23" max="23" width="12.7109375" customWidth="true"/>
+    <col min="38" max="38" width="10.7109375" customWidth="true"/>
+    <col min="39" max="39" width="12.7109375" customWidth="true"/>
+    <col min="3" max="3" width="12.7109375" customWidth="true"/>
+    <col min="4" max="4" width="12.7109375" customWidth="true"/>
+    <col min="5" max="5" width="12.7109375" customWidth="true"/>
+    <col min="6" max="6" width="12.7109375" customWidth="true"/>
+    <col min="7" max="7" width="12.7109375" customWidth="true"/>
+    <col min="8" max="8" width="12.7109375" customWidth="true"/>
+    <col min="9" max="9" width="12.7109375" customWidth="true"/>
+    <col min="10" max="10" width="12.7109375" customWidth="true"/>
+    <col min="11" max="11" width="12.7109375" customWidth="true"/>
+    <col min="12" max="12" width="12.7109375" customWidth="true"/>
+    <col min="13" max="13" width="12.7109375" customWidth="true"/>
+    <col min="14" max="14" width="12.7109375" customWidth="true"/>
+    <col min="15" max="15" width="12.7109375" customWidth="true"/>
+    <col min="16" max="16" width="12.7109375" customWidth="true"/>
+    <col min="17" max="17" width="12.7109375" customWidth="true"/>
+    <col min="18" max="18" width="12.7109375" customWidth="true"/>
+    <col min="19" max="19" width="12.7109375" customWidth="true"/>
+    <col min="20" max="20" width="12.7109375" customWidth="true"/>
+    <col min="21" max="21" width="12.7109375" customWidth="true"/>
+    <col min="24" max="24" width="12.7109375" customWidth="true"/>
+    <col min="25" max="25" width="12.7109375" customWidth="true"/>
+    <col min="26" max="26" width="12.7109375" customWidth="true"/>
+    <col min="27" max="27" width="12.7109375" customWidth="true"/>
+    <col min="28" max="28" width="12.7109375" customWidth="true"/>
+    <col min="29" max="29" width="12.7109375" customWidth="true"/>
+    <col min="30" max="30" width="12.7109375" customWidth="true"/>
+    <col min="31" max="31" width="12.7109375" customWidth="true"/>
+    <col min="32" max="32" width="12.7109375" customWidth="true"/>
+    <col min="33" max="33" width="12.7109375" customWidth="true"/>
+    <col min="34" max="34" width="12.7109375" customWidth="true"/>
+    <col min="35" max="35" width="12.7109375" customWidth="true"/>
+    <col min="36" max="36" width="12.7109375" customWidth="true"/>
+    <col min="37" max="37" width="12.7109375" customWidth="true"/>
+    <col min="40" max="40" width="12.7109375" customWidth="true"/>
+    <col min="41" max="41" width="12.7109375" customWidth="true"/>
+    <col min="42" max="42" width="12.7109375" customWidth="true"/>
+    <col min="43" max="43" width="12.7109375" customWidth="true"/>
+    <col min="44" max="44" width="12.7109375" customWidth="true"/>
+    <col min="45" max="45" width="12.7109375" customWidth="true"/>
+    <col min="46" max="46" width="12.7109375" customWidth="true"/>
+    <col min="47" max="47" width="12.7109375" customWidth="true"/>
+    <col min="48" max="48" width="12.7109375" customWidth="true"/>
+    <col min="49" max="49" width="12.7109375" customWidth="true"/>
+    <col min="50" max="50" width="12.7109375" customWidth="true"/>
+    <col min="51" max="51" width="12.7109375" customWidth="true"/>
+    <col min="52" max="52" width="12.7109375" customWidth="true"/>
+    <col min="53" max="53" width="12.7109375" customWidth="true"/>
+    <col min="54" max="54" width="12.7109375" customWidth="true"/>
+    <col min="55" max="55" width="12.7109375" customWidth="true"/>
+    <col min="56" max="56" width="12.7109375" customWidth="true"/>
+    <col min="57" max="57" width="12.7109375" customWidth="true"/>
+    <col min="58" max="58" width="12.7109375" customWidth="true"/>
+    <col min="59" max="59" width="12.7109375" customWidth="true"/>
+    <col min="60" max="60" width="12.7109375" customWidth="true"/>
+    <col min="61" max="61" width="12.7109375" customWidth="true"/>
+    <col min="62" max="62" width="12.7109375" customWidth="true"/>
+    <col min="63" max="63" width="12.7109375" customWidth="true"/>
+    <col min="64" max="64" width="12.7109375" customWidth="true"/>
+    <col min="65" max="65" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AP1" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AR1" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AT1" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AU1" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AW1" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AX1" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AY1" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BA1" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BB1" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BC1" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BD1" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BE1" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BF1" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BG1" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BH1" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BI1" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BK1" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BL1" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BM1" s="2" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="U2" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="V2" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="X2" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Y2" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="Z2" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AA2" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AB2" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AC2" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AD2" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AE2" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AF2" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AG2" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AH2" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AI2" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AK2" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AL2" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AM2" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AN2" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AO2" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="AP2" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AR2" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AS2" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AT2" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AU2" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AV2" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AW2" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="AX2" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="AY2" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="AZ2" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="BA2" s="1" t="s">
+      <c r="BA2" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="BB2" s="1" t="s">
+      <c r="BB2" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="BC2" s="1" t="s">
+      <c r="BC2" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="BD2" s="1" t="s">
+      <c r="BD2" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="BE2" s="1" t="s">
+      <c r="BE2" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="BF2" s="1" t="s">
+      <c r="BF2" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="BG2" s="1" t="s">
+      <c r="BG2" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="BH2" s="1" t="s">
+      <c r="BH2" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="BI2" s="1" t="s">
+      <c r="BI2" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="BJ2" s="1" t="s">
+      <c r="BJ2" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="BK2" s="1" t="s">
+      <c r="BK2" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="BL2" s="1" t="s">
+      <c r="BL2" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="BM2" s="1" t="s">
+      <c r="BM2" s="2" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="U3" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="V3" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="W3" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="X3" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Y3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="Z3" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AA3" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AB3" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AC3" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AD3" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AE3" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AF3" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AG3" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="AH3" s="1" t="s">
+      <c r="AH3" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="AI3" s="1" t="s">
+      <c r="AI3" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="AJ3" s="1" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="AK3" s="1" t="s">
+      <c r="AK3" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="AL3" s="1" t="s">
+      <c r="AL3" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="AM3" s="1" t="s">
+      <c r="AM3" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="AN3" s="1" t="s">
+      <c r="AN3" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="AO3" s="1" t="s">
+      <c r="AO3" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="AP3" s="1" t="s">
+      <c r="AP3" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="AQ3" s="1" t="s">
+      <c r="AQ3" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="AR3" s="1" t="s">
+      <c r="AR3" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="AS3" s="1" t="s">
+      <c r="AS3" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="AT3" s="1" t="s">
+      <c r="AT3" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="AU3" s="1" t="s">
+      <c r="AU3" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="AV3" s="1" t="s">
+      <c r="AV3" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="AW3" s="1" t="s">
+      <c r="AW3" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="AX3" s="1" t="s">
+      <c r="AX3" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="AY3" s="1" t="s">
+      <c r="AY3" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="AZ3" s="1" t="s">
+      <c r="AZ3" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="BA3" s="1" t="s">
+      <c r="BA3" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="BB3" s="1" t="s">
+      <c r="BB3" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="BC3" s="1" t="s">
+      <c r="BC3" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="BD3" s="1" t="s">
+      <c r="BD3" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="BE3" s="1" t="s">
+      <c r="BE3" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="BF3" s="1" t="s">
+      <c r="BF3" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="BG3" s="1" t="s">
+      <c r="BG3" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="BH3" s="1" t="s">
+      <c r="BH3" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="BI3" s="1" t="s">
+      <c r="BI3" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="BJ3" s="1" t="s">
+      <c r="BJ3" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="BK3" s="1" t="s">
+      <c r="BK3" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="BL3" s="1" t="s">
+      <c r="BL3" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="BM3" s="1" t="s">
+      <c r="BM3" s="2" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="R4" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="S4" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="T4" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="U4" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="V4" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="W4" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="X4" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="Y4" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="Z4" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AA4" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AB4" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="AC4" s="1" t="s">
+      <c r="AC4" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AD4" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AE4" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AF4" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="AG4" s="1" t="s">
+      <c r="AG4" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="AH4" s="1" t="s">
+      <c r="AH4" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="AI4" s="1" t="s">
+      <c r="AI4" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="AJ4" s="1" t="s">
+      <c r="AJ4" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="AK4" s="1" t="s">
+      <c r="AK4" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="AL4" s="1" t="s">
+      <c r="AL4" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="AM4" s="1" t="s">
+      <c r="AM4" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="AN4" s="1" t="s">
+      <c r="AN4" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="AO4" s="1" t="s">
+      <c r="AO4" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AP4" s="1" t="s">
+      <c r="AP4" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="AQ4" s="1" t="s">
+      <c r="AQ4" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="AR4" s="1" t="s">
+      <c r="AR4" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="AS4" s="1" t="s">
+      <c r="AS4" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="AT4" s="1" t="s">
+      <c r="AT4" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="AU4" s="1" t="s">
+      <c r="AU4" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="AV4" s="1" t="s">
+      <c r="AV4" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="AW4" s="1" t="s">
+      <c r="AW4" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="AX4" s="1" t="s">
+      <c r="AX4" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="AY4" s="1" t="s">
+      <c r="AY4" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="AZ4" s="1" t="s">
+      <c r="AZ4" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="BA4" s="1" t="s">
+      <c r="BA4" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="BB4" s="1" t="s">
+      <c r="BB4" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="BC4" s="1" t="s">
+      <c r="BC4" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="BD4" s="1" t="s">
+      <c r="BD4" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="BE4" s="1" t="s">
+      <c r="BE4" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="BF4" s="1" t="s">
+      <c r="BF4" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="BG4" s="1" t="s">
+      <c r="BG4" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="BH4" s="1" t="s">
+      <c r="BH4" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="BI4" s="1" t="s">
+      <c r="BI4" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="BJ4" s="1" t="s">
+      <c r="BJ4" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="BK4" s="1" t="s">
+      <c r="BK4" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="BL4" s="1" t="s">
+      <c r="BL4" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="BM4" s="1" t="s">
+      <c r="BM4" s="2" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="R5" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="S5" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="T5" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="U5" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="V5" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="W5" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="X5" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="Y5" s="1" t="s">
+      <c r="Y5" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="Z5" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AA5" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="AB5" s="1" t="s">
+      <c r="AB5" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="AC5" s="1" t="s">
+      <c r="AC5" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AD5" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="AE5" s="1" t="s">
+      <c r="AE5" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="AF5" s="1" t="s">
+      <c r="AF5" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="AG5" s="1" t="s">
+      <c r="AG5" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="AH5" s="1" t="s">
+      <c r="AH5" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="AI5" s="1" t="s">
+      <c r="AI5" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="AJ5" s="1" t="s">
+      <c r="AJ5" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="AK5" s="1" t="s">
+      <c r="AK5" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="AL5" s="1" t="s">
+      <c r="AL5" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="AM5" s="1" t="s">
+      <c r="AM5" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="AN5" s="1" t="s">
+      <c r="AN5" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="AO5" s="1" t="s">
+      <c r="AO5" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="AP5" s="1" t="s">
+      <c r="AP5" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="AQ5" s="1" t="s">
+      <c r="AQ5" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="AR5" s="1" t="s">
+      <c r="AR5" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="AS5" s="1" t="s">
+      <c r="AS5" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="AT5" s="1" t="s">
+      <c r="AT5" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="AU5" s="1" t="s">
+      <c r="AU5" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="AV5" s="1" t="s">
+      <c r="AV5" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="AW5" s="1" t="s">
+      <c r="AW5" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="AX5" s="1" t="s">
+      <c r="AX5" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="AY5" s="1" t="s">
+      <c r="AY5" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="AZ5" s="1" t="s">
+      <c r="AZ5" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="BA5" s="1" t="s">
+      <c r="BA5" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="BB5" s="1" t="s">
+      <c r="BB5" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="BC5" s="1" t="s">
+      <c r="BC5" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="BD5" s="1" t="s">
+      <c r="BD5" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="BE5" s="1" t="s">
+      <c r="BE5" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="BF5" s="1" t="s">
+      <c r="BF5" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="BG5" s="1" t="s">
+      <c r="BG5" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="BH5" s="1" t="s">
+      <c r="BH5" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="BI5" s="1" t="s">
+      <c r="BI5" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="BJ5" s="1" t="s">
+      <c r="BJ5" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="BK5" s="1" t="s">
+      <c r="BK5" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="BL5" s="1" t="s">
+      <c r="BL5" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="BM5" s="1" t="s">
+      <c r="BM5" s="2" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="R6" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="S6" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="T6" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="U6" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="V6" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="W6" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="X6" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="Y6" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="Z6" s="1" t="s">
+      <c r="Z6" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AA6" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="AB6" s="1" t="s">
+      <c r="AB6" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="AC6" s="1" t="s">
+      <c r="AC6" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AD6" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="AE6" s="1" t="s">
+      <c r="AE6" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="AF6" s="1" t="s">
+      <c r="AF6" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="AG6" s="1" t="s">
+      <c r="AG6" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="AH6" s="1" t="s">
+      <c r="AH6" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="AI6" s="1" t="s">
+      <c r="AI6" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="AJ6" s="1" t="s">
+      <c r="AJ6" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="AK6" s="1" t="s">
+      <c r="AK6" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="AL6" s="1" t="s">
+      <c r="AL6" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="AM6" s="1" t="s">
+      <c r="AM6" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="AN6" s="1" t="s">
+      <c r="AN6" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="AO6" s="1" t="s">
+      <c r="AO6" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="AP6" s="1" t="s">
+      <c r="AP6" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="AQ6" s="1" t="s">
+      <c r="AQ6" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="AR6" s="1" t="s">
+      <c r="AR6" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="AS6" s="1" t="s">
+      <c r="AS6" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="AT6" s="1" t="s">
+      <c r="AT6" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="AU6" s="1" t="s">
+      <c r="AU6" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="AV6" s="1" t="s">
+      <c r="AV6" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="AW6" s="1" t="s">
+      <c r="AW6" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="AX6" s="1" t="s">
+      <c r="AX6" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="AY6" s="1" t="s">
+      <c r="AY6" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="AZ6" s="1" t="s">
+      <c r="AZ6" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="BA6" s="1" t="s">
+      <c r="BA6" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="BB6" s="1" t="s">
+      <c r="BB6" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="BC6" s="1" t="s">
+      <c r="BC6" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="BD6" s="1" t="s">
+      <c r="BD6" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="BE6" s="1" t="s">
+      <c r="BE6" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="BF6" s="1" t="s">
+      <c r="BF6" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="BG6" s="1" t="s">
+      <c r="BG6" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="BH6" s="1" t="s">
+      <c r="BH6" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="BI6" s="1" t="s">
+      <c r="BI6" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="BJ6" s="1" t="s">
+      <c r="BJ6" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="BK6" s="1" t="s">
+      <c r="BK6" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="BL6" s="1" t="s">
+      <c r="BL6" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="BM6" s="1" t="s">
+      <c r="BM6" s="2" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="R7" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="S7" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="T7" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="U7" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="V7" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="W7" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="X7" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="Y7" s="1" t="s">
+      <c r="Y7" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="Z7" s="1" t="s">
+      <c r="Z7" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AA7" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AB7" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="AC7" s="1" t="s">
+      <c r="AC7" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AD7" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="AE7" s="1" t="s">
+      <c r="AE7" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="AF7" s="1" t="s">
+      <c r="AF7" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="AG7" s="1" t="s">
+      <c r="AG7" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="AH7" s="1" t="s">
+      <c r="AH7" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="AI7" s="1" t="s">
+      <c r="AI7" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="AJ7" s="1" t="s">
+      <c r="AJ7" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="AK7" s="1" t="s">
+      <c r="AK7" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="AL7" s="1" t="s">
+      <c r="AL7" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="AM7" s="1" t="s">
+      <c r="AM7" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="AN7" s="1" t="s">
+      <c r="AN7" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="AO7" s="1" t="s">
+      <c r="AO7" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="AP7" s="1" t="s">
+      <c r="AP7" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="AQ7" s="1" t="s">
+      <c r="AQ7" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="AR7" s="1" t="s">
+      <c r="AR7" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="AS7" s="1" t="s">
+      <c r="AS7" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="AT7" s="1" t="s">
+      <c r="AT7" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="AU7" s="1" t="s">
+      <c r="AU7" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="AV7" s="1" t="s">
+      <c r="AV7" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="AW7" s="1" t="s">
+      <c r="AW7" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="AX7" s="1" t="s">
+      <c r="AX7" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="AY7" s="1" t="s">
+      <c r="AY7" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="AZ7" s="1" t="s">
+      <c r="AZ7" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="BA7" s="1" t="s">
+      <c r="BA7" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="BB7" s="1" t="s">
+      <c r="BB7" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="BC7" s="1" t="s">
+      <c r="BC7" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="BD7" s="1" t="s">
+      <c r="BD7" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="BE7" s="1" t="s">
+      <c r="BE7" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="BF7" s="1" t="s">
+      <c r="BF7" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="BG7" s="1" t="s">
+      <c r="BG7" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="BH7" s="1" t="s">
+      <c r="BH7" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="BI7" s="1" t="s">
+      <c r="BI7" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="BJ7" s="1" t="s">
+      <c r="BJ7" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="BK7" s="1" t="s">
+      <c r="BK7" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="BL7" s="1" t="s">
+      <c r="BL7" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="BM7" s="1" t="s">
+      <c r="BM7" s="2" t="s">
         <v>411</v>
       </c>
     </row>
@@ -3015,24 +3064,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added gui and improved data selection
</commit_message>
<xml_diff>
--- a/Codon optimization/data_formatted.xlsx
+++ b/Codon optimization/data_formatted.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2990" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6175" uniqueCount="461">
   <si>
     <t>combined1</t>
   </si>
@@ -1252,6 +1252,153 @@
   </si>
   <si>
     <t>13540.5</t>
+  </si>
+  <si>
+    <t>12321</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>19</t>
   </si>
 </sst>
 </file>
@@ -1272,7 +1419,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1299,11 +1446,27 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1318,6 +1481,22 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1700,1382 +1879,1382 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="R1" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="V1" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="W1" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="X1" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="Y1" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="Z1" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="AA1" s="12" t="s">
+      <c r="AA1" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="AB1" s="12" t="s">
+      <c r="AB1" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="AC1" s="12" t="s">
+      <c r="AC1" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="AD1" s="12" t="s">
+      <c r="AD1" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="AE1" s="12" t="s">
+      <c r="AE1" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="AF1" s="12" t="s">
+      <c r="AF1" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="AG1" s="12" t="s">
+      <c r="AG1" s="28" t="s">
         <v>206</v>
       </c>
-      <c r="AH1" s="12" t="s">
+      <c r="AH1" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="AI1" s="12" t="s">
+      <c r="AI1" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="AJ1" s="12" t="s">
+      <c r="AJ1" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="AK1" s="12" t="s">
+      <c r="AK1" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="AL1" s="12" t="s">
+      <c r="AL1" s="28" t="s">
         <v>237</v>
       </c>
-      <c r="AM1" s="12" t="s">
+      <c r="AM1" s="28" t="s">
         <v>244</v>
       </c>
-      <c r="AN1" s="12" t="s">
+      <c r="AN1" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="AO1" s="12" t="s">
+      <c r="AO1" s="28" t="s">
         <v>256</v>
       </c>
-      <c r="AP1" s="12" t="s">
+      <c r="AP1" s="28" t="s">
         <v>262</v>
       </c>
-      <c r="AQ1" s="12" t="s">
+      <c r="AQ1" s="28" t="s">
         <v>269</v>
       </c>
-      <c r="AR1" s="12" t="s">
+      <c r="AR1" s="28" t="s">
         <v>275</v>
       </c>
-      <c r="AS1" s="12" t="s">
+      <c r="AS1" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="AT1" s="12" t="s">
+      <c r="AT1" s="28" t="s">
         <v>287</v>
       </c>
-      <c r="AU1" s="12" t="s">
+      <c r="AU1" s="28" t="s">
         <v>294</v>
       </c>
-      <c r="AV1" s="12" t="s">
+      <c r="AV1" s="28" t="s">
         <v>300</v>
       </c>
-      <c r="AW1" s="12" t="s">
+      <c r="AW1" s="28" t="s">
         <v>306</v>
       </c>
-      <c r="AX1" s="12" t="s">
+      <c r="AX1" s="28" t="s">
         <v>312</v>
       </c>
-      <c r="AY1" s="12" t="s">
+      <c r="AY1" s="28" t="s">
         <v>319</v>
       </c>
-      <c r="AZ1" s="12" t="s">
+      <c r="AZ1" s="28" t="s">
         <v>325</v>
       </c>
-      <c r="BA1" s="12" t="s">
+      <c r="BA1" s="28" t="s">
         <v>331</v>
       </c>
-      <c r="BB1" s="12" t="s">
+      <c r="BB1" s="28" t="s">
         <v>338</v>
       </c>
-      <c r="BC1" s="12" t="s">
+      <c r="BC1" s="28" t="s">
         <v>345</v>
       </c>
-      <c r="BD1" s="12" t="s">
+      <c r="BD1" s="28" t="s">
         <v>351</v>
       </c>
-      <c r="BE1" s="12" t="s">
+      <c r="BE1" s="28" t="s">
         <v>357</v>
       </c>
-      <c r="BF1" s="12" t="s">
+      <c r="BF1" s="28" t="s">
         <v>363</v>
       </c>
-      <c r="BG1" s="12" t="s">
+      <c r="BG1" s="28" t="s">
         <v>369</v>
       </c>
-      <c r="BH1" s="12" t="s">
+      <c r="BH1" s="28" t="s">
         <v>375</v>
       </c>
-      <c r="BI1" s="12" t="s">
+      <c r="BI1" s="28" t="s">
         <v>381</v>
       </c>
-      <c r="BJ1" s="12" t="s">
+      <c r="BJ1" s="28" t="s">
         <v>387</v>
       </c>
-      <c r="BK1" s="12" t="s">
+      <c r="BK1" s="28" t="s">
         <v>394</v>
       </c>
-      <c r="BL1" s="12" t="s">
+      <c r="BL1" s="28" t="s">
         <v>400</v>
       </c>
-      <c r="BM1" s="12" t="s">
+      <c r="BM1" s="28" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="P2" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q2" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="R2" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="S2" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="T2" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="U2" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="V2" s="12" t="s">
+      <c r="V2" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="W2" s="12" t="s">
+      <c r="W2" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="X2" s="12" t="s">
+      <c r="X2" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="Y2" s="12" t="s">
+      <c r="Y2" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="Z2" s="12" t="s">
+      <c r="Z2" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="AA2" s="12" t="s">
+      <c r="AA2" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="AB2" s="12" t="s">
+      <c r="AB2" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="AC2" s="12" t="s">
+      <c r="AC2" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="AD2" s="12" t="s">
+      <c r="AD2" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="AE2" s="12" t="s">
+      <c r="AE2" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="AF2" s="12" t="s">
+      <c r="AF2" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="AG2" s="12" t="s">
+      <c r="AG2" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="AH2" s="12" t="s">
+      <c r="AH2" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="AI2" s="12" t="s">
+      <c r="AI2" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="AJ2" s="12" t="s">
+      <c r="AJ2" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="AK2" s="12" t="s">
+      <c r="AK2" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="AL2" s="12" t="s">
+      <c r="AL2" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="AM2" s="12" t="s">
+      <c r="AM2" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="AN2" s="12" t="s">
+      <c r="AN2" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="AO2" s="12" t="s">
+      <c r="AO2" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="AP2" s="12" t="s">
+      <c r="AP2" s="28" t="s">
         <v>263</v>
       </c>
-      <c r="AQ2" s="12" t="s">
+      <c r="AQ2" s="28" t="s">
         <v>263</v>
       </c>
-      <c r="AR2" s="12" t="s">
+      <c r="AR2" s="28" t="s">
         <v>263</v>
       </c>
-      <c r="AS2" s="12" t="s">
+      <c r="AS2" s="28" t="s">
         <v>263</v>
       </c>
-      <c r="AT2" s="12" t="s">
+      <c r="AT2" s="28" t="s">
         <v>288</v>
       </c>
-      <c r="AU2" s="12" t="s">
+      <c r="AU2" s="28" t="s">
         <v>288</v>
       </c>
-      <c r="AV2" s="12" t="s">
+      <c r="AV2" s="28" t="s">
         <v>288</v>
       </c>
-      <c r="AW2" s="12" t="s">
+      <c r="AW2" s="28" t="s">
         <v>288</v>
       </c>
-      <c r="AX2" s="12" t="s">
+      <c r="AX2" s="28" t="s">
         <v>313</v>
       </c>
-      <c r="AY2" s="12" t="s">
+      <c r="AY2" s="28" t="s">
         <v>313</v>
       </c>
-      <c r="AZ2" s="12" t="s">
+      <c r="AZ2" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="BA2" s="12" t="s">
+      <c r="BA2" s="28" t="s">
         <v>332</v>
       </c>
-      <c r="BB2" s="12" t="s">
+      <c r="BB2" s="28" t="s">
         <v>339</v>
       </c>
-      <c r="BC2" s="12" t="s">
+      <c r="BC2" s="28" t="s">
         <v>339</v>
       </c>
-      <c r="BD2" s="12" t="s">
+      <c r="BD2" s="28" t="s">
         <v>339</v>
       </c>
-      <c r="BE2" s="12" t="s">
+      <c r="BE2" s="28" t="s">
         <v>339</v>
       </c>
-      <c r="BF2" s="12" t="s">
+      <c r="BF2" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="BG2" s="12" t="s">
+      <c r="BG2" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="BH2" s="12" t="s">
+      <c r="BH2" s="28" t="s">
         <v>339</v>
       </c>
-      <c r="BI2" s="12" t="s">
+      <c r="BI2" s="28" t="s">
         <v>339</v>
       </c>
-      <c r="BJ2" s="12" t="s">
+      <c r="BJ2" s="28" t="s">
         <v>388</v>
       </c>
-      <c r="BK2" s="12" t="s">
+      <c r="BK2" s="28" t="s">
         <v>388</v>
       </c>
-      <c r="BL2" s="12" t="s">
+      <c r="BL2" s="28" t="s">
         <v>388</v>
       </c>
-      <c r="BM2" s="12" t="s">
+      <c r="BM2" s="28" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="T3" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="U3" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="V3" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="W3" s="12" t="s">
+      <c r="W3" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="X3" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="Y3" s="12" t="s">
+      <c r="Y3" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="Z3" s="12" t="s">
+      <c r="Z3" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AA3" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="AB3" s="12" t="s">
+      <c r="AB3" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="AC3" s="12" t="s">
+      <c r="AC3" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="AD3" s="12" t="s">
+      <c r="AD3" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="AE3" s="12" t="s">
+      <c r="AE3" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="AF3" s="12" t="s">
+      <c r="AF3" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="AG3" s="12" t="s">
+      <c r="AG3" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="AH3" s="12" t="s">
+      <c r="AH3" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="AI3" s="12" t="s">
+      <c r="AI3" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="AJ3" s="12" t="s">
+      <c r="AJ3" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="AK3" s="12" t="s">
+      <c r="AK3" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="AL3" s="12" t="s">
+      <c r="AL3" s="28" t="s">
         <v>239</v>
       </c>
-      <c r="AM3" s="12" t="s">
+      <c r="AM3" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AN3" s="12" t="s">
+      <c r="AN3" s="28" t="s">
         <v>251</v>
       </c>
-      <c r="AO3" s="12" t="s">
+      <c r="AO3" s="28" t="s">
         <v>257</v>
       </c>
-      <c r="AP3" s="12" t="s">
+      <c r="AP3" s="28" t="s">
         <v>264</v>
       </c>
-      <c r="AQ3" s="12" t="s">
+      <c r="AQ3" s="28" t="s">
         <v>270</v>
       </c>
-      <c r="AR3" s="12" t="s">
+      <c r="AR3" s="28" t="s">
         <v>276</v>
       </c>
-      <c r="AS3" s="12" t="s">
+      <c r="AS3" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="AT3" s="12" t="s">
+      <c r="AT3" s="28" t="s">
         <v>289</v>
       </c>
-      <c r="AU3" s="12" t="s">
+      <c r="AU3" s="28" t="s">
         <v>295</v>
       </c>
-      <c r="AV3" s="12" t="s">
+      <c r="AV3" s="28" t="s">
         <v>301</v>
       </c>
-      <c r="AW3" s="12" t="s">
+      <c r="AW3" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="AX3" s="12" t="s">
+      <c r="AX3" s="28" t="s">
         <v>314</v>
       </c>
-      <c r="AY3" s="12" t="s">
+      <c r="AY3" s="28" t="s">
         <v>320</v>
       </c>
-      <c r="AZ3" s="12" t="s">
+      <c r="AZ3" s="28" t="s">
         <v>326</v>
       </c>
-      <c r="BA3" s="12" t="s">
+      <c r="BA3" s="28" t="s">
         <v>333</v>
       </c>
-      <c r="BB3" s="12" t="s">
+      <c r="BB3" s="28" t="s">
         <v>340</v>
       </c>
-      <c r="BC3" s="12" t="s">
+      <c r="BC3" s="28" t="s">
         <v>346</v>
       </c>
-      <c r="BD3" s="12" t="s">
+      <c r="BD3" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="BE3" s="12" t="s">
+      <c r="BE3" s="28" t="s">
         <v>358</v>
       </c>
-      <c r="BF3" s="12" t="s">
+      <c r="BF3" s="28" t="s">
         <v>364</v>
       </c>
-      <c r="BG3" s="12" t="s">
+      <c r="BG3" s="28" t="s">
         <v>370</v>
       </c>
-      <c r="BH3" s="12" t="s">
+      <c r="BH3" s="28" t="s">
         <v>376</v>
       </c>
-      <c r="BI3" s="12" t="s">
+      <c r="BI3" s="28" t="s">
         <v>382</v>
       </c>
-      <c r="BJ3" s="12" t="s">
+      <c r="BJ3" s="28" t="s">
         <v>389</v>
       </c>
-      <c r="BK3" s="12" t="s">
+      <c r="BK3" s="28" t="s">
         <v>395</v>
       </c>
-      <c r="BL3" s="12" t="s">
+      <c r="BL3" s="28" t="s">
         <v>401</v>
       </c>
-      <c r="BM3" s="12" t="s">
+      <c r="BM3" s="28" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="M4" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="O4" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="P4" s="12" t="s">
+      <c r="P4" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="Q4" s="12" t="s">
+      <c r="Q4" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="R4" s="12" t="s">
+      <c r="R4" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="S4" s="12" t="s">
+      <c r="S4" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="T4" s="12" t="s">
+      <c r="T4" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="U4" s="12" t="s">
+      <c r="U4" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="V4" s="12" t="s">
+      <c r="V4" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="W4" s="12" t="s">
+      <c r="W4" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="X4" s="12" t="s">
+      <c r="X4" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="Y4" s="12" t="s">
+      <c r="Y4" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="Z4" s="12" t="s">
+      <c r="Z4" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="AA4" s="12" t="s">
+      <c r="AA4" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="AB4" s="12" t="s">
+      <c r="AB4" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="AC4" s="12" t="s">
+      <c r="AC4" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="AD4" s="12" t="s">
+      <c r="AD4" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="AE4" s="12" t="s">
+      <c r="AE4" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="AF4" s="12" t="s">
+      <c r="AF4" s="28" t="s">
         <v>202</v>
       </c>
-      <c r="AG4" s="12" t="s">
+      <c r="AG4" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="AH4" s="12" t="s">
+      <c r="AH4" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="AI4" s="12" t="s">
+      <c r="AI4" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="AJ4" s="12" t="s">
+      <c r="AJ4" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="AK4" s="12" t="s">
+      <c r="AK4" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="AL4" s="12" t="s">
+      <c r="AL4" s="28" t="s">
         <v>240</v>
       </c>
-      <c r="AM4" s="12" t="s">
+      <c r="AM4" s="28" t="s">
         <v>246</v>
       </c>
-      <c r="AN4" s="12" t="s">
+      <c r="AN4" s="28" t="s">
         <v>252</v>
       </c>
-      <c r="AO4" s="12" t="s">
+      <c r="AO4" s="28" t="s">
         <v>258</v>
       </c>
-      <c r="AP4" s="12" t="s">
+      <c r="AP4" s="28" t="s">
         <v>265</v>
       </c>
-      <c r="AQ4" s="12" t="s">
+      <c r="AQ4" s="28" t="s">
         <v>271</v>
       </c>
-      <c r="AR4" s="12" t="s">
+      <c r="AR4" s="28" t="s">
         <v>277</v>
       </c>
-      <c r="AS4" s="12" t="s">
+      <c r="AS4" s="28" t="s">
         <v>283</v>
       </c>
-      <c r="AT4" s="12" t="s">
+      <c r="AT4" s="28" t="s">
         <v>290</v>
       </c>
-      <c r="AU4" s="12" t="s">
+      <c r="AU4" s="28" t="s">
         <v>296</v>
       </c>
-      <c r="AV4" s="12" t="s">
+      <c r="AV4" s="28" t="s">
         <v>302</v>
       </c>
-      <c r="AW4" s="12" t="s">
+      <c r="AW4" s="28" t="s">
         <v>308</v>
       </c>
-      <c r="AX4" s="12" t="s">
+      <c r="AX4" s="28" t="s">
         <v>315</v>
       </c>
-      <c r="AY4" s="12" t="s">
+      <c r="AY4" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="AZ4" s="12" t="s">
+      <c r="AZ4" s="28" t="s">
         <v>327</v>
       </c>
-      <c r="BA4" s="12" t="s">
+      <c r="BA4" s="28" t="s">
         <v>334</v>
       </c>
-      <c r="BB4" s="12" t="s">
+      <c r="BB4" s="28" t="s">
         <v>341</v>
       </c>
-      <c r="BC4" s="12" t="s">
+      <c r="BC4" s="28" t="s">
         <v>347</v>
       </c>
-      <c r="BD4" s="12" t="s">
+      <c r="BD4" s="28" t="s">
         <v>353</v>
       </c>
-      <c r="BE4" s="12" t="s">
+      <c r="BE4" s="28" t="s">
         <v>359</v>
       </c>
-      <c r="BF4" s="12" t="s">
+      <c r="BF4" s="28" t="s">
         <v>365</v>
       </c>
-      <c r="BG4" s="12" t="s">
+      <c r="BG4" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="BH4" s="12" t="s">
+      <c r="BH4" s="28" t="s">
         <v>377</v>
       </c>
-      <c r="BI4" s="12" t="s">
+      <c r="BI4" s="28" t="s">
         <v>383</v>
       </c>
-      <c r="BJ4" s="12" t="s">
+      <c r="BJ4" s="28" t="s">
         <v>390</v>
       </c>
-      <c r="BK4" s="12" t="s">
+      <c r="BK4" s="28" t="s">
         <v>396</v>
       </c>
-      <c r="BL4" s="12" t="s">
+      <c r="BL4" s="28" t="s">
         <v>402</v>
       </c>
-      <c r="BM4" s="12" t="s">
+      <c r="BM4" s="28" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="P5" s="12" t="s">
+      <c r="P5" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="Q5" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="R5" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="S5" s="12" t="s">
+      <c r="S5" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="T5" s="12" t="s">
+      <c r="T5" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="U5" s="12" t="s">
+      <c r="U5" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="V5" s="12" t="s">
+      <c r="V5" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="W5" s="12" t="s">
+      <c r="W5" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="X5" s="12" t="s">
+      <c r="X5" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="Y5" s="12" t="s">
+      <c r="Y5" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="Z5" s="12" t="s">
+      <c r="Z5" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="AA5" s="12" t="s">
+      <c r="AA5" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="AB5" s="12" t="s">
+      <c r="AB5" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="AC5" s="12" t="s">
+      <c r="AC5" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="AD5" s="12" t="s">
+      <c r="AD5" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="AE5" s="12" t="s">
+      <c r="AE5" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="AF5" s="12" t="s">
+      <c r="AF5" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="AG5" s="12" t="s">
+      <c r="AG5" s="28" t="s">
         <v>210</v>
       </c>
-      <c r="AH5" s="12" t="s">
+      <c r="AH5" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="AI5" s="12" t="s">
+      <c r="AI5" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="AJ5" s="12" t="s">
+      <c r="AJ5" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="AK5" s="12" t="s">
+      <c r="AK5" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="AL5" s="12" t="s">
+      <c r="AL5" s="28" t="s">
         <v>242</v>
       </c>
-      <c r="AM5" s="12" t="s">
+      <c r="AM5" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="AN5" s="12" t="s">
+      <c r="AN5" s="28" t="s">
         <v>254</v>
       </c>
-      <c r="AO5" s="12" t="s">
+      <c r="AO5" s="28" t="s">
         <v>260</v>
       </c>
-      <c r="AP5" s="12" t="s">
+      <c r="AP5" s="28" t="s">
         <v>267</v>
       </c>
-      <c r="AQ5" s="12" t="s">
+      <c r="AQ5" s="28" t="s">
         <v>273</v>
       </c>
-      <c r="AR5" s="12" t="s">
+      <c r="AR5" s="28" t="s">
         <v>279</v>
       </c>
-      <c r="AS5" s="12" t="s">
+      <c r="AS5" s="28" t="s">
         <v>285</v>
       </c>
-      <c r="AT5" s="12" t="s">
+      <c r="AT5" s="28" t="s">
         <v>292</v>
       </c>
-      <c r="AU5" s="12" t="s">
+      <c r="AU5" s="28" t="s">
         <v>298</v>
       </c>
-      <c r="AV5" s="12" t="s">
+      <c r="AV5" s="28" t="s">
         <v>304</v>
       </c>
-      <c r="AW5" s="12" t="s">
+      <c r="AW5" s="28" t="s">
         <v>310</v>
       </c>
-      <c r="AX5" s="12" t="s">
+      <c r="AX5" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="AY5" s="12" t="s">
+      <c r="AY5" s="28" t="s">
         <v>323</v>
       </c>
-      <c r="AZ5" s="12" t="s">
+      <c r="AZ5" s="28" t="s">
         <v>329</v>
       </c>
-      <c r="BA5" s="12" t="s">
+      <c r="BA5" s="28" t="s">
         <v>336</v>
       </c>
-      <c r="BB5" s="12" t="s">
+      <c r="BB5" s="28" t="s">
         <v>343</v>
       </c>
-      <c r="BC5" s="12" t="s">
+      <c r="BC5" s="28" t="s">
         <v>349</v>
       </c>
-      <c r="BD5" s="12" t="s">
+      <c r="BD5" s="28" t="s">
         <v>355</v>
       </c>
-      <c r="BE5" s="12" t="s">
+      <c r="BE5" s="28" t="s">
         <v>361</v>
       </c>
-      <c r="BF5" s="12" t="s">
+      <c r="BF5" s="28" t="s">
         <v>367</v>
       </c>
-      <c r="BG5" s="12" t="s">
+      <c r="BG5" s="28" t="s">
         <v>373</v>
       </c>
-      <c r="BH5" s="12" t="s">
+      <c r="BH5" s="28" t="s">
         <v>379</v>
       </c>
-      <c r="BI5" s="12" t="s">
+      <c r="BI5" s="28" t="s">
         <v>385</v>
       </c>
-      <c r="BJ5" s="12" t="s">
+      <c r="BJ5" s="28" t="s">
         <v>392</v>
       </c>
-      <c r="BK5" s="12" t="s">
+      <c r="BK5" s="28" t="s">
         <v>398</v>
       </c>
-      <c r="BL5" s="12" t="s">
+      <c r="BL5" s="28" t="s">
         <v>404</v>
       </c>
-      <c r="BM5" s="12" t="s">
+      <c r="BM5" s="28" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="O6" s="12" t="s">
+      <c r="O6" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="P6" s="12" t="s">
+      <c r="P6" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="Q6" s="12" t="s">
+      <c r="Q6" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="R6" s="12" t="s">
+      <c r="R6" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="S6" s="12" t="s">
+      <c r="S6" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="T6" s="12" t="s">
+      <c r="T6" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="U6" s="12" t="s">
+      <c r="U6" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="V6" s="12" t="s">
+      <c r="V6" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="W6" s="12" t="s">
+      <c r="W6" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="X6" s="12" t="s">
+      <c r="X6" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="Y6" s="12" t="s">
+      <c r="Y6" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="Z6" s="12" t="s">
+      <c r="Z6" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="AA6" s="12" t="s">
+      <c r="AA6" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="AB6" s="12" t="s">
+      <c r="AB6" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="AC6" s="12" t="s">
+      <c r="AC6" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="AD6" s="12" t="s">
+      <c r="AD6" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="AE6" s="12" t="s">
+      <c r="AE6" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="AF6" s="12" t="s">
+      <c r="AF6" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="AG6" s="12" t="s">
+      <c r="AG6" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="AH6" s="12" t="s">
+      <c r="AH6" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="AI6" s="12" t="s">
+      <c r="AI6" s="28" t="s">
         <v>224</v>
       </c>
-      <c r="AJ6" s="12" t="s">
+      <c r="AJ6" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="AK6" s="12" t="s">
+      <c r="AK6" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="AL6" s="12" t="s">
+      <c r="AL6" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="AM6" s="12" t="s">
+      <c r="AM6" s="28" t="s">
         <v>249</v>
       </c>
-      <c r="AN6" s="12" t="s">
+      <c r="AN6" s="28" t="s">
         <v>255</v>
       </c>
-      <c r="AO6" s="12" t="s">
+      <c r="AO6" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="AP6" s="12" t="s">
+      <c r="AP6" s="28" t="s">
         <v>268</v>
       </c>
-      <c r="AQ6" s="12" t="s">
+      <c r="AQ6" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="AR6" s="12" t="s">
+      <c r="AR6" s="28" t="s">
         <v>280</v>
       </c>
-      <c r="AS6" s="12" t="s">
+      <c r="AS6" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="AT6" s="12" t="s">
+      <c r="AT6" s="28" t="s">
         <v>293</v>
       </c>
-      <c r="AU6" s="12" t="s">
+      <c r="AU6" s="28" t="s">
         <v>299</v>
       </c>
-      <c r="AV6" s="12" t="s">
+      <c r="AV6" s="28" t="s">
         <v>305</v>
       </c>
-      <c r="AW6" s="12" t="s">
+      <c r="AW6" s="28" t="s">
         <v>311</v>
       </c>
-      <c r="AX6" s="12" t="s">
+      <c r="AX6" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="AY6" s="12" t="s">
+      <c r="AY6" s="28" t="s">
         <v>324</v>
       </c>
-      <c r="AZ6" s="12" t="s">
+      <c r="AZ6" s="28" t="s">
         <v>330</v>
       </c>
-      <c r="BA6" s="12" t="s">
+      <c r="BA6" s="28" t="s">
         <v>337</v>
       </c>
-      <c r="BB6" s="12" t="s">
+      <c r="BB6" s="28" t="s">
         <v>344</v>
       </c>
-      <c r="BC6" s="12" t="s">
+      <c r="BC6" s="28" t="s">
         <v>350</v>
       </c>
-      <c r="BD6" s="12" t="s">
+      <c r="BD6" s="28" t="s">
         <v>356</v>
       </c>
-      <c r="BE6" s="12" t="s">
+      <c r="BE6" s="28" t="s">
         <v>362</v>
       </c>
-      <c r="BF6" s="12" t="s">
+      <c r="BF6" s="28" t="s">
         <v>368</v>
       </c>
-      <c r="BG6" s="12" t="s">
+      <c r="BG6" s="28" t="s">
         <v>374</v>
       </c>
-      <c r="BH6" s="12" t="s">
+      <c r="BH6" s="28" t="s">
         <v>380</v>
       </c>
-      <c r="BI6" s="12" t="s">
+      <c r="BI6" s="28" t="s">
         <v>386</v>
       </c>
-      <c r="BJ6" s="12" t="s">
+      <c r="BJ6" s="28" t="s">
         <v>393</v>
       </c>
-      <c r="BK6" s="12" t="s">
+      <c r="BK6" s="28" t="s">
         <v>399</v>
       </c>
-      <c r="BL6" s="12" t="s">
+      <c r="BL6" s="28" t="s">
         <v>405</v>
       </c>
-      <c r="BM6" s="12" t="s">
+      <c r="BM6" s="28" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="U7" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="V7" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="W7" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="X7" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="Y7" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="Z7" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="AA7" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="AB7" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="AC7" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="AD7" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="AE7" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="AF7" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="AG7" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="AH7" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="AI7" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="AJ7" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="AK7" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="AL7" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="AM7" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="AN7" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="AO7" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="AP7" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="AQ7" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="AR7" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="AS7" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="AT7" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="AU7" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="AV7" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="AW7" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="AX7" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="AY7" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="AZ7" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="BA7" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="BB7" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="BC7" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="BD7" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="BE7" s="6" t="s">
-        <v>362</v>
-      </c>
-      <c r="BF7" s="6" t="s">
-        <v>368</v>
-      </c>
-      <c r="BG7" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="BH7" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="BI7" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="BJ7" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="BK7" s="6" t="s">
-        <v>399</v>
-      </c>
-      <c r="BL7" s="6" t="s">
-        <v>405</v>
-      </c>
-      <c r="BM7" s="6" t="s">
-        <v>411</v>
+      <c r="A7" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>416</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>417</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>418</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>419</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>421</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="M7" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="N7" s="18" t="s">
+        <v>425</v>
+      </c>
+      <c r="O7" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="P7" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q7" s="18" t="s">
+        <v>427</v>
+      </c>
+      <c r="R7" s="18" t="s">
+        <v>428</v>
+      </c>
+      <c r="S7" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="T7" s="18" t="s">
+        <v>429</v>
+      </c>
+      <c r="U7" s="18" t="s">
+        <v>430</v>
+      </c>
+      <c r="V7" s="18" t="s">
+        <v>431</v>
+      </c>
+      <c r="W7" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="X7" s="18" t="s">
+        <v>433</v>
+      </c>
+      <c r="Y7" s="18" t="s">
+        <v>434</v>
+      </c>
+      <c r="Z7" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="AA7" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="AB7" s="18" t="s">
+        <v>435</v>
+      </c>
+      <c r="AC7" s="18" t="s">
+        <v>436</v>
+      </c>
+      <c r="AD7" s="18" t="s">
+        <v>437</v>
+      </c>
+      <c r="AE7" s="18" t="s">
+        <v>428</v>
+      </c>
+      <c r="AF7" s="18" t="s">
+        <v>438</v>
+      </c>
+      <c r="AG7" s="18" t="s">
+        <v>439</v>
+      </c>
+      <c r="AH7" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="AI7" s="18" t="s">
+        <v>441</v>
+      </c>
+      <c r="AJ7" s="18" t="s">
+        <v>442</v>
+      </c>
+      <c r="AK7" s="18" t="s">
+        <v>443</v>
+      </c>
+      <c r="AL7" s="18" t="s">
+        <v>444</v>
+      </c>
+      <c r="AM7" s="18" t="s">
+        <v>445</v>
+      </c>
+      <c r="AN7" s="18" t="s">
+        <v>446</v>
+      </c>
+      <c r="AO7" s="18" t="s">
+        <v>447</v>
+      </c>
+      <c r="AP7" s="18" t="s">
+        <v>448</v>
+      </c>
+      <c r="AQ7" s="18" t="s">
+        <v>445</v>
+      </c>
+      <c r="AR7" s="18" t="s">
+        <v>449</v>
+      </c>
+      <c r="AS7" s="18" t="s">
+        <v>450</v>
+      </c>
+      <c r="AT7" s="18" t="s">
+        <v>448</v>
+      </c>
+      <c r="AU7" s="18" t="s">
+        <v>451</v>
+      </c>
+      <c r="AV7" s="18" t="s">
+        <v>452</v>
+      </c>
+      <c r="AW7" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="AX7" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="AY7" s="18" t="s">
+        <v>418</v>
+      </c>
+      <c r="AZ7" s="18" t="s">
+        <v>453</v>
+      </c>
+      <c r="BA7" s="18" t="s">
+        <v>454</v>
+      </c>
+      <c r="BB7" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="BC7" s="18" t="s">
+        <v>455</v>
+      </c>
+      <c r="BD7" s="18" t="s">
+        <v>447</v>
+      </c>
+      <c r="BE7" s="18" t="s">
+        <v>456</v>
+      </c>
+      <c r="BF7" s="18" t="s">
+        <v>434</v>
+      </c>
+      <c r="BG7" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="BH7" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="BI7" s="18" t="s">
+        <v>457</v>
+      </c>
+      <c r="BJ7" s="18" t="s">
+        <v>425</v>
+      </c>
+      <c r="BK7" s="18" t="s">
+        <v>458</v>
+      </c>
+      <c r="BL7" s="18" t="s">
+        <v>459</v>
+      </c>
+      <c r="BM7" s="18" t="s">
+        <v>460</v>
       </c>
     </row>
   </sheetData>

</xml_diff>